<commit_message>
modif tableau de synthèse
</commit_message>
<xml_diff>
--- a/cv tableau_synthese pp/Tableau_de_synthèse_Epreuve_E4_2025.xlsx
+++ b/cv tableau_synthese pp/Tableau_de_synthèse_Epreuve_E4_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lyceeort-my.sharepoint.com/personal/aaron_edery_ortmontreuil_fr/Documents/Bureau/Portfolio et note de synthèse/Portfolio/cv tableau_synthese pp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="13_ncr:1_{CD607C19-8393-1147-9752-9B89A961AAD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{522642B1-4225-46D4-B73C-611FD9F91B1E}"/>
+  <xr:revisionPtr revIDLastSave="91" documentId="13_ncr:1_{CD607C19-8393-1147-9752-9B89A961AAD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A11DC2C8-0581-4C9D-956F-0C434E64E226}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
   <si>
     <t>Gérer le patrimoine informatique</t>
   </si>
@@ -110,9 +110,6 @@
     <t>Réalisations en milieu professionnel en cours de seconde année</t>
   </si>
   <si>
-    <t>Adresse URL du portfolio :</t>
-  </si>
-  <si>
     <t>SESSION 2025</t>
   </si>
   <si>
@@ -144,6 +141,18 @@
   </si>
   <si>
     <t>Apprentissage de diverses frameworks Python</t>
+  </si>
+  <si>
+    <t>Veliko partie java</t>
+  </si>
+  <si>
+    <t>LinkedIn</t>
+  </si>
+  <si>
+    <t>Gestion des données de l'entreprise</t>
+  </si>
+  <si>
+    <t>Adresse URL du portfolio : https://aedery16-11.github.io/edery.github.io/</t>
   </si>
 </sst>
 </file>
@@ -611,7 +620,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -667,6 +676,60 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -694,59 +757,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -764,6 +776,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>136715</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>70868</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>469504</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>488789</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Image 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8716DC2B-66B8-B2E9-D62E-5060006B7F2B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12325837" y="1605301"/>
+          <a:ext cx="332789" cy="417921"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1058,8 +1119,8 @@
   </sheetPr>
   <dimension ref="A1:AQ81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="70" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="67" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1072,56 +1133,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="19"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="37"/>
     </row>
     <row r="2" spans="1:43" ht="41" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
     </row>
     <row r="3" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="26" t="s">
+      <c r="A3" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="21"/>
-      <c r="H3" s="27"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="39"/>
+      <c r="H3" s="45"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="25"/>
+      <c r="A4" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="43"/>
       <c r="F4" s="12" t="s">
         <v>8</v>
       </c>
@@ -1133,22 +1194,22 @@
       </c>
     </row>
     <row r="5" spans="1:43" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="32"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="33"/>
+      <c r="A5" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="36"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="32" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -1169,26 +1230,27 @@
       <c r="H6" s="7" t="s">
         <v>5</v>
       </c>
+      <c r="J6" s="46"/>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="325" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="42"/>
-      <c r="B7" s="30"/>
-      <c r="C7" s="44" t="s">
+      <c r="A7" s="24"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="44" t="s">
+      <c r="D7" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="44" t="s">
+      <c r="E7" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="44" t="s">
+      <c r="F7" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="44" t="s">
+      <c r="G7" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="45" t="s">
+      <c r="H7" s="22" t="s">
         <v>14</v>
       </c>
       <c r="I7"/>
@@ -1228,16 +1290,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="40"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="41"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="28"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1276,13 +1338,13 @@
     </row>
     <row r="9" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="35" t="s">
-        <v>28</v>
+      <c r="C9" s="20" t="s">
+        <v>27</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
@@ -1327,18 +1389,18 @@
     </row>
     <row r="10" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10" s="14"/>
       <c r="D10" s="14"/>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
-      <c r="H10" s="34" t="s">
-        <v>28</v>
+      <c r="H10" s="19" t="s">
+        <v>27</v>
       </c>
       <c r="I10"/>
       <c r="J10"/>
@@ -1378,23 +1440,23 @@
     </row>
     <row r="11" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C11" s="14"/>
-      <c r="D11" s="34" t="s">
-        <v>28</v>
+      <c r="D11" s="19" t="s">
+        <v>27</v>
       </c>
       <c r="E11" s="14"/>
-      <c r="F11" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="G11" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="H11" s="34"/>
+      <c r="F11" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="H11" s="19"/>
       <c r="I11"/>
       <c r="J11"/>
       <c r="K11"/>
@@ -1432,14 +1494,24 @@
       <c r="AQ11"/>
     </row>
     <row r="12" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="8"/>
+      <c r="A12" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>30</v>
+      </c>
       <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
+      <c r="D12" s="19" t="s">
+        <v>27</v>
+      </c>
       <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="15"/>
+      <c r="F12" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="H12" s="19"/>
       <c r="I12"/>
       <c r="J12"/>
       <c r="K12"/>
@@ -1477,13 +1549,20 @@
       <c r="AQ12"/>
     </row>
     <row r="13" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="8"/>
+      <c r="A13" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="8">
+        <v>2023</v>
+      </c>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
-      <c r="H13" s="15"/>
+      <c r="H13" s="19" t="s">
+        <v>27</v>
+      </c>
       <c r="I13"/>
       <c r="J13"/>
       <c r="K13"/>
@@ -1746,16 +1825,16 @@
       <c r="AQ18"/>
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A19" s="36" t="s">
+      <c r="A19" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="38"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="31"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -1794,7 +1873,7 @@
     </row>
     <row r="20" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B20" s="8">
         <v>2024</v>
@@ -1802,14 +1881,14 @@
       <c r="C20" s="14"/>
       <c r="D20" s="14"/>
       <c r="E20" s="14"/>
-      <c r="F20" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="G20" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="H20" s="34" t="s">
-        <v>28</v>
+      <c r="F20" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="G20" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="H20" s="19" t="s">
+        <v>27</v>
       </c>
       <c r="I20"/>
       <c r="J20"/>
@@ -1849,7 +1928,7 @@
     </row>
     <row r="21" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B21" s="8">
         <v>2024</v>
@@ -1859,8 +1938,8 @@
       <c r="E21" s="14"/>
       <c r="F21" s="14"/>
       <c r="G21" s="14"/>
-      <c r="H21" s="34" t="s">
-        <v>28</v>
+      <c r="H21" s="19" t="s">
+        <v>27</v>
       </c>
       <c r="I21"/>
       <c r="J21"/>
@@ -1899,12 +1978,18 @@
       <c r="AQ21"/>
     </row>
     <row r="22" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="9"/>
-      <c r="B22" s="8"/>
+      <c r="A22" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="8">
+        <v>2024</v>
+      </c>
       <c r="C22" s="14"/>
       <c r="D22" s="14"/>
       <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
+      <c r="F22" s="19" t="s">
+        <v>27</v>
+      </c>
       <c r="G22" s="14"/>
       <c r="H22" s="15"/>
       <c r="I22"/>
@@ -2124,16 +2209,16 @@
       <c r="AQ26"/>
     </row>
     <row r="27" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="38"/>
+      <c r="B27" s="30"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="31"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2578,6 +2663,11 @@
     <row r="81" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
@@ -2585,16 +2675,12 @@
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="9" scale="48" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
mise à jour du tableau de synthèse
</commit_message>
<xml_diff>
--- a/cv tableau_synthese pp/Tableau_de_synthèse_Epreuve_E4_2025.xlsx
+++ b/cv tableau_synthese pp/Tableau_de_synthèse_Epreuve_E4_2025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lyceeort-my.sharepoint.com/personal/aaron_edery_ortmontreuil_fr/Documents/Bureau/Portfolio et note de synthèse/Portfolio/cv tableau_synthese pp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="91" documentId="13_ncr:1_{CD607C19-8393-1147-9752-9B89A961AAD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A11DC2C8-0581-4C9D-956F-0C434E64E226}"/>
+  <xr:revisionPtr revIDLastSave="107" documentId="13_ncr:1_{CD607C19-8393-1147-9752-9B89A961AAD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4EF28E9-2C21-46CB-A698-9005374DF103}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
   <si>
     <t>Gérer le patrimoine informatique</t>
   </si>
@@ -153,6 +153,18 @@
   </si>
   <si>
     <t>Adresse URL du portfolio : https://aedery16-11.github.io/edery.github.io/</t>
+  </si>
+  <si>
+    <t>Développement d’un script d’analyse des assets</t>
+  </si>
+  <si>
+    <t>2024-2025</t>
+  </si>
+  <si>
+    <t>Création de visualisations pour l’analyse des données</t>
+  </si>
+  <si>
+    <t>Adaptation et correction du script en fonction des retours</t>
   </si>
 </sst>
 </file>
@@ -162,7 +174,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* &quot;-&quot;??\ [$€-1]_-"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -224,6 +236,18 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -620,7 +644,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -688,6 +712,36 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -730,35 +784,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1119,70 +1149,70 @@
   </sheetPr>
   <dimension ref="A1:AQ81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="67" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="67" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="70.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.81640625" style="1" customWidth="1"/>
-    <col min="3" max="8" width="18.6328125" style="1" customWidth="1"/>
-    <col min="9" max="43" width="10.90625" customWidth="1"/>
-    <col min="44" max="16384" width="10.81640625" style="1"/>
+    <col min="1" max="1" width="70.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" style="1" customWidth="1"/>
+    <col min="3" max="8" width="18.5703125" style="1" customWidth="1"/>
+    <col min="9" max="43" width="10.85546875" customWidth="1"/>
+    <col min="44" max="16384" width="10.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="37"/>
-    </row>
-    <row r="2" spans="1:43" ht="41" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="25" t="s">
+      <c r="H1" s="24"/>
+    </row>
+    <row r="2" spans="1:43" ht="41.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-    </row>
-    <row r="3" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+    </row>
+    <row r="3" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="44" t="s">
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="39"/>
-      <c r="H3" s="45"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="32"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="41" t="s">
+    <row r="4" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="43"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="30"/>
       <c r="F4" s="12" t="s">
         <v>8</v>
       </c>
@@ -1193,23 +1223,23 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:43" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="34" t="s">
+    <row r="5" spans="1:43" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="36"/>
-    </row>
-    <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
+      <c r="B5" s="45"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="46"/>
+    </row>
+    <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="42" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -1230,11 +1260,11 @@
       <c r="H6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="46"/>
-    </row>
-    <row r="7" spans="1:43" s="2" customFormat="1" ht="325" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="24"/>
-      <c r="B7" s="33"/>
+      <c r="J6" s="23"/>
+    </row>
+    <row r="7" spans="1:43" s="2" customFormat="1" ht="324.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="34"/>
+      <c r="B7" s="43"/>
       <c r="C7" s="21" t="s">
         <v>9</v>
       </c>
@@ -1289,17 +1319,17 @@
       <c r="AP7"/>
       <c r="AQ7"/>
     </row>
-    <row r="8" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
+    <row r="8" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A8" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="28"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="38"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1336,7 +1366,7 @@
       <c r="AP8"/>
       <c r="AQ8"/>
     </row>
-    <row r="9" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>29</v>
       </c>
@@ -1387,7 +1417,7 @@
       <c r="AP9"/>
       <c r="AQ9"/>
     </row>
-    <row r="10" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
         <v>26</v>
       </c>
@@ -1438,7 +1468,7 @@
       <c r="AP10"/>
       <c r="AQ10"/>
     </row>
-    <row r="11" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
         <v>28</v>
       </c>
@@ -1493,7 +1523,7 @@
       <c r="AP11"/>
       <c r="AQ11"/>
     </row>
-    <row r="12" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
         <v>33</v>
       </c>
@@ -1548,7 +1578,7 @@
       <c r="AP12"/>
       <c r="AQ12"/>
     </row>
-    <row r="13" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>34</v>
       </c>
@@ -1599,7 +1629,7 @@
       <c r="AP13"/>
       <c r="AQ13"/>
     </row>
-    <row r="14" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="9"/>
       <c r="B14" s="8"/>
       <c r="C14" s="14"/>
@@ -1644,7 +1674,7 @@
       <c r="AP14"/>
       <c r="AQ14"/>
     </row>
-    <row r="15" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="9"/>
       <c r="B15" s="8"/>
       <c r="C15" s="14"/>
@@ -1689,7 +1719,7 @@
       <c r="AP15"/>
       <c r="AQ15"/>
     </row>
-    <row r="16" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="9"/>
       <c r="B16" s="8"/>
       <c r="C16" s="14"/>
@@ -1734,7 +1764,7 @@
       <c r="AP16"/>
       <c r="AQ16"/>
     </row>
-    <row r="17" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="9"/>
       <c r="B17" s="8"/>
       <c r="C17" s="14"/>
@@ -1779,7 +1809,7 @@
       <c r="AP17"/>
       <c r="AQ17"/>
     </row>
-    <row r="18" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="9"/>
       <c r="B18" s="8"/>
       <c r="C18" s="14"/>
@@ -1824,17 +1854,17 @@
       <c r="AP18"/>
       <c r="AQ18"/>
     </row>
-    <row r="19" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A19" s="29" t="s">
+    <row r="19" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A19" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="30"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="30"/>
-      <c r="G19" s="30"/>
-      <c r="H19" s="31"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="41"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -1871,7 +1901,7 @@
       <c r="AP19"/>
       <c r="AQ19"/>
     </row>
-    <row r="20" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
         <v>31</v>
       </c>
@@ -1926,7 +1956,7 @@
       <c r="AP20"/>
       <c r="AQ20"/>
     </row>
-    <row r="21" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
         <v>32</v>
       </c>
@@ -1977,7 +2007,7 @@
       <c r="AP21"/>
       <c r="AQ21"/>
     </row>
-    <row r="22" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
         <v>35</v>
       </c>
@@ -2028,7 +2058,7 @@
       <c r="AP22"/>
       <c r="AQ22"/>
     </row>
-    <row r="23" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="9"/>
       <c r="B23" s="8"/>
       <c r="C23" s="14"/>
@@ -2073,7 +2103,7 @@
       <c r="AP23"/>
       <c r="AQ23"/>
     </row>
-    <row r="24" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="9"/>
       <c r="B24" s="8"/>
       <c r="C24" s="14"/>
@@ -2118,7 +2148,7 @@
       <c r="AP24"/>
       <c r="AQ24"/>
     </row>
-    <row r="25" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="9"/>
       <c r="B25" s="8"/>
       <c r="C25" s="14"/>
@@ -2163,7 +2193,7 @@
       <c r="AP25"/>
       <c r="AQ25"/>
     </row>
-    <row r="26" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="9"/>
       <c r="B26" s="8"/>
       <c r="C26" s="14"/>
@@ -2208,17 +2238,17 @@
       <c r="AP26"/>
       <c r="AQ26"/>
     </row>
-    <row r="27" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A27" s="29" t="s">
+    <row r="27" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A27" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="30"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="30"/>
-      <c r="H27" s="31"/>
+      <c r="B27" s="40"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="40"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="40"/>
+      <c r="G27" s="40"/>
+      <c r="H27" s="41"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2255,10 +2285,16 @@
       <c r="AP27"/>
       <c r="AQ27"/>
     </row>
-    <row r="28" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="9"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="14"/>
+    <row r="28" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" s="20" t="s">
+        <v>27</v>
+      </c>
       <c r="D28" s="14"/>
       <c r="E28" s="14"/>
       <c r="F28" s="14"/>
@@ -2300,13 +2336,17 @@
       <c r="AP28"/>
       <c r="AQ28"/>
     </row>
-    <row r="29" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="9"/>
+    <row r="29" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="48" t="s">
+        <v>39</v>
+      </c>
       <c r="B29" s="8"/>
       <c r="C29" s="14"/>
       <c r="D29" s="14"/>
       <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
+      <c r="F29" s="20" t="s">
+        <v>27</v>
+      </c>
       <c r="G29" s="14"/>
       <c r="H29" s="15"/>
       <c r="I29"/>
@@ -2345,11 +2385,15 @@
       <c r="AP29"/>
       <c r="AQ29"/>
     </row>
-    <row r="30" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="9"/>
+    <row r="30" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="48" t="s">
+        <v>40</v>
+      </c>
       <c r="B30" s="8"/>
       <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
+      <c r="D30" s="20" t="s">
+        <v>27</v>
+      </c>
       <c r="E30" s="14"/>
       <c r="F30" s="14"/>
       <c r="G30" s="14"/>
@@ -2390,7 +2434,7 @@
       <c r="AP30"/>
       <c r="AQ30"/>
     </row>
-    <row r="31" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="9"/>
       <c r="B31" s="8"/>
       <c r="C31" s="14"/>
@@ -2435,7 +2479,7 @@
       <c r="AP31"/>
       <c r="AQ31"/>
     </row>
-    <row r="32" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="9"/>
       <c r="B32" s="8"/>
       <c r="C32" s="14"/>
@@ -2480,7 +2524,7 @@
       <c r="AP32"/>
       <c r="AQ32"/>
     </row>
-    <row r="33" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="9"/>
       <c r="B33" s="8"/>
       <c r="C33" s="14"/>
@@ -2525,7 +2569,7 @@
       <c r="AP33"/>
       <c r="AQ33"/>
     </row>
-    <row r="34" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="10"/>
       <c r="B34" s="11"/>
       <c r="C34" s="16"/>
@@ -2570,7 +2614,7 @@
       <c r="AP34"/>
       <c r="AQ34"/>
     </row>
-    <row r="35" spans="1:43" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:43" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="5"/>
       <c r="B35" s="3"/>
       <c r="C35" s="4"/>
@@ -2615,59 +2659,54 @@
       <c r="AP35"/>
       <c r="AQ35"/>
     </row>
-    <row r="36" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="55" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="56" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="57" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="58" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="59" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="60" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="61" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="62" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="63" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="64" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="65" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="66" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="67" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="68" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="69" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="70" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="71" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="72" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="73" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="74" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="75" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="76" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="77" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="78" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="79" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="80" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="81" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="55" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="56" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="57" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="58" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="59" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="60" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="61" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="62" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="63" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="64" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="65" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="66" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="67" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="68" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="69" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="70" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="71" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="72" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="73" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="74" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="75" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="76" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="77" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="78" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="79" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="80" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="81" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
@@ -2675,6 +2714,11 @@
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>